<commit_message>
fayoumi (add course module)
</commit_message>
<xml_diff>
--- a/test_data/changePasswordIfMatched.xlsx
+++ b/test_data/changePasswordIfMatched.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CYBORG\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Test Automation\Kalemon\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCBF61FB-7857-44CE-81B3-A61953541B24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0859E113-4C90-4BAE-BA98-35DC36741F9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Phone_Number</t>
   </si>
@@ -46,6 +46,9 @@
   </si>
   <si>
     <t>Kalemon@</t>
+  </si>
+  <si>
+    <t>790000017</t>
   </si>
 </sst>
 </file>
@@ -90,7 +93,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -99,6 +102,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -385,7 +391,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -411,8 +417,8 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="1">
-        <v>790000017</v>
+      <c r="A2" s="4" t="s">
+        <v>7</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>4</v>

</xml_diff>